<commit_message>
Changed to enter amount and quantity away from cases and lbs. Seems to be working but needs more testing
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/CUST03.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/CUST03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\AutoBlueSystemSrc\customer_product_codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980A5E11-648F-475E-9D22-16DD241E46A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC0F86-BA48-457B-887D-15798284E0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="2190" windowWidth="31935" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="3825" windowWidth="31935" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>1 p1fett case</t>
-  </si>
-  <si>
     <t>1 case spinach fettuccine</t>
   </si>
   <si>
     <t>2 egg papp</t>
   </si>
   <si>
-    <t>2 p2papp lbs</t>
+    <t>1 p1fett 4E</t>
+  </si>
+  <si>
+    <t>2 p2papp 5E</t>
   </si>
 </sst>
 </file>
@@ -357,22 +357,22 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fixed auto enter issue. Added deletion checks
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/CUST03.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/CUST03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\AutoBlueSystemSrc\customer_product_codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC0F86-BA48-457B-887D-15798284E0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EE8310-6949-4209-8C23-A07815A962D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="3825" windowWidth="31935" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>1 case spinach fettuccine</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>2 p2papp 5E</t>
+  </si>
+  <si>
+    <t>5 Spinach Linguine</t>
+  </si>
+  <si>
+    <t>5 SPLING 4E</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,6 +384,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>